<commit_message>
Updated model results summary - com mods
</commit_message>
<xml_diff>
--- a/Results/Macroeconomics/macroecon_models.xlsx
+++ b/Results/Macroeconomics/macroecon_models.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\PhD_Chapter1\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\PhD_Chapter1\Results\Macroeconomics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="me.mods" sheetId="1" r:id="rId1"/>
+    <sheet name="com.mods" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
   <si>
     <t>MACROECONOMIC SET</t>
   </si>
@@ -138,14 +139,76 @@
   </si>
   <si>
     <t>% more</t>
+  </si>
+  <si>
+    <t>COMMODITY SET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model </t>
+  </si>
+  <si>
+    <t>com.mod3</t>
+  </si>
+  <si>
+    <t>armi</t>
+  </si>
+  <si>
+    <t>rice_med</t>
+  </si>
+  <si>
+    <t>com.mod4</t>
+  </si>
+  <si>
+    <t>com.mod5</t>
+  </si>
+  <si>
+    <t>1-YEAR LAG</t>
+  </si>
+  <si>
+    <t>for_prod</t>
+  </si>
+  <si>
+    <t>rub_med</t>
+  </si>
+  <si>
+    <t>com.modlag.2</t>
+  </si>
+  <si>
+    <t>com.glmlag.1</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>inverse</t>
+  </si>
+  <si>
+    <t>model AIC</t>
+  </si>
+  <si>
+    <t>com.glmlag.2</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>com.glmlag.3</t>
+  </si>
+  <si>
+    <t>identity</t>
+  </si>
+  <si>
+    <t>resid.dev/df</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="170" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -175,7 +238,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,6 +269,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -219,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -249,6 +318,28 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,12 +1294,13 @@
         <v>26.930342384887837</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I34" s="10"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>6</v>
       </c>
@@ -1222,7 +1314,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>-501.3</v>
       </c>
@@ -1240,6 +1332,310 @@
       <c r="F36">
         <f>E36-100</f>
         <v>4.5501695591383395E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="6"/>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="7"/>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2.6539999999999999</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="E6" s="4">
+        <v>6.0229999999999999E-2</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1.075</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.97850000000000004</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2">
+        <v>268.45999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3.056</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4">
+        <v>6.0429999999999998E-2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1.073</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.97889999999999999</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2">
+        <v>265.45999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.2591</v>
+      </c>
+      <c r="E8" s="4">
+        <v>5.9499999999999997E-2</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1.075</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.97729999999999995</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="17">
+        <v>-1.6579999999999999E-4</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3.2919999999999998E-2</v>
+      </c>
+      <c r="E12" s="4">
+        <v>5.645E-2</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.99609999999999999</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.98060000000000003</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2">
+        <v>254.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="20">
+        <v>8.6140000000000004E-10</v>
+      </c>
+      <c r="D13" s="18">
+        <v>-1.8659999999999999E-7</v>
+      </c>
+      <c r="E13" s="20">
+        <v>-9.383E-8</v>
+      </c>
+      <c r="F13" s="21">
+        <v>-1.057E-6</v>
+      </c>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="3">
+        <v>1.07</v>
+      </c>
+      <c r="J13" s="19"/>
+      <c r="K13">
+        <v>324.77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="22">
+        <v>-6.7179999999999997E-7</v>
+      </c>
+      <c r="D14" s="22">
+        <v>1.4770000000000001E-4</v>
+      </c>
+      <c r="E14" s="23">
+        <v>8.551E-5</v>
+      </c>
+      <c r="F14" s="23">
+        <v>1.217E-3</v>
+      </c>
+      <c r="I14">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="K14">
+        <v>321.85000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="25">
+        <v>-6.1269999999999999E-4</v>
+      </c>
+      <c r="D15" s="25">
+        <v>5.4870000000000002E-2</v>
+      </c>
+      <c r="E15" s="23">
+        <v>6.6919999999999993E-2</v>
+      </c>
+      <c r="F15" s="23">
+        <v>0.95209999999999995</v>
+      </c>
+      <c r="G15" s="24"/>
+      <c r="I15" s="26">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="K15">
+        <v>245.85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>